<commit_message>
Minor change allows autofill to column `MQ_Experiment` in `expt_smry.xlsx`
</commit_message>
<xml_diff>
--- a/inst/extdata/expt_smry_cptac_gl_mq.xlsx
+++ b/inst/extdata/expt_smry_cptac_gl_mq.xlsx
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="131">
   <si>
     <t>Description</t>
   </si>
@@ -1938,9 +1938,9 @@
   <dimension ref="A1:V61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2096,9 +2096,7 @@
       <c r="D3" s="15"/>
       <c r="E3" s="16"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G3" s="18"/>
       <c r="H3" s="17" t="s">
         <v>51</v>
       </c>
@@ -2144,9 +2142,7 @@
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G4" s="18"/>
       <c r="H4" s="14" t="s">
         <v>42</v>
       </c>
@@ -2192,9 +2188,7 @@
       <c r="D5" s="15"/>
       <c r="E5" s="16"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G5" s="18"/>
       <c r="H5" s="14" t="s">
         <v>43</v>
       </c>
@@ -2240,9 +2234,7 @@
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G6" s="18"/>
       <c r="H6" s="14" t="s">
         <v>52</v>
       </c>
@@ -2288,9 +2280,7 @@
       <c r="D7" s="15"/>
       <c r="E7" s="16"/>
       <c r="F7" s="18"/>
-      <c r="G7" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G7" s="18"/>
       <c r="H7" s="14" t="s">
         <v>44</v>
       </c>
@@ -2336,9 +2326,7 @@
       <c r="D8" s="15"/>
       <c r="E8" s="16"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G8" s="18"/>
       <c r="H8" s="14" t="s">
         <v>53</v>
       </c>
@@ -2384,9 +2372,7 @@
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
       <c r="F9" s="18"/>
-      <c r="G9" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G9" s="18"/>
       <c r="H9" s="14" t="s">
         <v>54</v>
       </c>
@@ -2432,9 +2418,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="18"/>
-      <c r="G10" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G10" s="18"/>
       <c r="H10" s="28" t="s">
         <v>45</v>
       </c>
@@ -2480,9 +2464,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
       <c r="F11" s="18"/>
-      <c r="G11" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="G11" s="18"/>
       <c r="H11" s="28" t="s">
         <v>55</v>
       </c>
@@ -2580,9 +2562,7 @@
       <c r="D13" s="34"/>
       <c r="E13" s="35"/>
       <c r="F13" s="37"/>
-      <c r="G13" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G13" s="37"/>
       <c r="H13" s="36" t="s">
         <v>56</v>
       </c>
@@ -2628,9 +2608,7 @@
       <c r="D14" s="34"/>
       <c r="E14" s="35"/>
       <c r="F14" s="37"/>
-      <c r="G14" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G14" s="37"/>
       <c r="H14" s="44" t="s">
         <v>47</v>
       </c>
@@ -2676,9 +2654,7 @@
       <c r="D15" s="34"/>
       <c r="E15" s="35"/>
       <c r="F15" s="37"/>
-      <c r="G15" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G15" s="37"/>
       <c r="H15" s="44" t="s">
         <v>48</v>
       </c>
@@ -2724,9 +2700,7 @@
       <c r="D16" s="34"/>
       <c r="E16" s="35"/>
       <c r="F16" s="37"/>
-      <c r="G16" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G16" s="37"/>
       <c r="H16" s="44" t="s">
         <v>57</v>
       </c>
@@ -2772,9 +2746,7 @@
       <c r="D17" s="34"/>
       <c r="E17" s="35"/>
       <c r="F17" s="37"/>
-      <c r="G17" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G17" s="37"/>
       <c r="H17" s="44" t="s">
         <v>49</v>
       </c>
@@ -2820,9 +2792,7 @@
       <c r="D18" s="34"/>
       <c r="E18" s="35"/>
       <c r="F18" s="37"/>
-      <c r="G18" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G18" s="37"/>
       <c r="H18" s="44" t="s">
         <v>58</v>
       </c>
@@ -2868,9 +2838,7 @@
       <c r="D19" s="34"/>
       <c r="E19" s="35"/>
       <c r="F19" s="37"/>
-      <c r="G19" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G19" s="37"/>
       <c r="H19" s="44" t="s">
         <v>59</v>
       </c>
@@ -2916,9 +2884,7 @@
       <c r="D20" s="34"/>
       <c r="E20" s="35"/>
       <c r="F20" s="37"/>
-      <c r="G20" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G20" s="37"/>
       <c r="H20" s="44" t="s">
         <v>50</v>
       </c>
@@ -2964,9 +2930,7 @@
       <c r="D21" s="34"/>
       <c r="E21" s="35"/>
       <c r="F21" s="37"/>
-      <c r="G21" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G21" s="37"/>
       <c r="H21" s="44" t="s">
         <v>60</v>
       </c>
@@ -3064,9 +3028,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="16"/>
       <c r="F23" s="18"/>
-      <c r="G23" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G23" s="18"/>
       <c r="H23" s="17" t="s">
         <v>96</v>
       </c>
@@ -3112,9 +3074,7 @@
       <c r="D24" s="15"/>
       <c r="E24" s="16"/>
       <c r="F24" s="18"/>
-      <c r="G24" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G24" s="18"/>
       <c r="H24" s="14" t="s">
         <v>99</v>
       </c>
@@ -3160,9 +3120,7 @@
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
       <c r="F25" s="18"/>
-      <c r="G25" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G25" s="18"/>
       <c r="H25" s="14" t="s">
         <v>100</v>
       </c>
@@ -3208,9 +3166,7 @@
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G26" s="18"/>
       <c r="H26" s="14" t="s">
         <v>101</v>
       </c>
@@ -3256,9 +3212,7 @@
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
       <c r="F27" s="18"/>
-      <c r="G27" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G27" s="18"/>
       <c r="H27" s="14" t="s">
         <v>102</v>
       </c>
@@ -3304,9 +3258,7 @@
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="18"/>
-      <c r="G28" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G28" s="18"/>
       <c r="H28" s="14" t="s">
         <v>103</v>
       </c>
@@ -3352,9 +3304,7 @@
       <c r="D29" s="15"/>
       <c r="E29" s="16"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G29" s="18"/>
       <c r="H29" s="14" t="s">
         <v>104</v>
       </c>
@@ -3400,9 +3350,7 @@
       <c r="D30" s="15"/>
       <c r="E30" s="16"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G30" s="18"/>
       <c r="H30" s="28" t="s">
         <v>105</v>
       </c>
@@ -3448,9 +3396,7 @@
       <c r="D31" s="15"/>
       <c r="E31" s="16"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="18" t="s">
-        <v>127</v>
-      </c>
+      <c r="G31" s="18"/>
       <c r="H31" s="28" t="s">
         <v>106</v>
       </c>
@@ -3548,9 +3494,7 @@
       <c r="D33" s="34"/>
       <c r="E33" s="35"/>
       <c r="F33" s="37"/>
-      <c r="G33" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G33" s="37"/>
       <c r="H33" s="36" t="s">
         <v>109</v>
       </c>
@@ -3596,9 +3540,7 @@
       <c r="D34" s="34"/>
       <c r="E34" s="35"/>
       <c r="F34" s="37"/>
-      <c r="G34" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G34" s="37"/>
       <c r="H34" s="44" t="s">
         <v>111</v>
       </c>
@@ -3644,9 +3586,7 @@
       <c r="D35" s="34"/>
       <c r="E35" s="35"/>
       <c r="F35" s="37"/>
-      <c r="G35" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G35" s="37"/>
       <c r="H35" s="44" t="s">
         <v>112</v>
       </c>
@@ -3692,9 +3632,7 @@
       <c r="D36" s="34"/>
       <c r="E36" s="35"/>
       <c r="F36" s="37"/>
-      <c r="G36" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G36" s="37"/>
       <c r="H36" s="44" t="s">
         <v>113</v>
       </c>
@@ -3740,9 +3678,7 @@
       <c r="D37" s="34"/>
       <c r="E37" s="35"/>
       <c r="F37" s="37"/>
-      <c r="G37" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G37" s="37"/>
       <c r="H37" s="44" t="s">
         <v>114</v>
       </c>
@@ -3788,9 +3724,7 @@
       <c r="D38" s="34"/>
       <c r="E38" s="35"/>
       <c r="F38" s="37"/>
-      <c r="G38" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G38" s="37"/>
       <c r="H38" s="44" t="s">
         <v>115</v>
       </c>
@@ -3836,9 +3770,7 @@
       <c r="D39" s="34"/>
       <c r="E39" s="35"/>
       <c r="F39" s="37"/>
-      <c r="G39" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G39" s="37"/>
       <c r="H39" s="44" t="s">
         <v>116</v>
       </c>
@@ -3884,9 +3816,7 @@
       <c r="D40" s="34"/>
       <c r="E40" s="35"/>
       <c r="F40" s="37"/>
-      <c r="G40" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G40" s="37"/>
       <c r="H40" s="44" t="s">
         <v>117</v>
       </c>
@@ -3932,9 +3862,7 @@
       <c r="D41" s="34"/>
       <c r="E41" s="35"/>
       <c r="F41" s="37"/>
-      <c r="G41" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G41" s="37"/>
       <c r="H41" s="44" t="s">
         <v>118</v>
       </c>
@@ -4032,9 +3960,7 @@
       <c r="D43" s="15"/>
       <c r="E43" s="16"/>
       <c r="F43" s="18"/>
-      <c r="G43" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G43" s="18"/>
       <c r="H43" s="17" t="s">
         <v>70</v>
       </c>
@@ -4080,9 +4006,7 @@
       <c r="D44" s="15"/>
       <c r="E44" s="16"/>
       <c r="F44" s="18"/>
-      <c r="G44" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G44" s="18"/>
       <c r="H44" s="14" t="s">
         <v>73</v>
       </c>
@@ -4128,9 +4052,7 @@
       <c r="D45" s="15"/>
       <c r="E45" s="16"/>
       <c r="F45" s="18"/>
-      <c r="G45" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G45" s="18"/>
       <c r="H45" s="14" t="s">
         <v>74</v>
       </c>
@@ -4176,9 +4098,7 @@
       <c r="D46" s="15"/>
       <c r="E46" s="16"/>
       <c r="F46" s="18"/>
-      <c r="G46" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G46" s="18"/>
       <c r="H46" s="14" t="s">
         <v>75</v>
       </c>
@@ -4224,9 +4144,7 @@
       <c r="D47" s="15"/>
       <c r="E47" s="16"/>
       <c r="F47" s="18"/>
-      <c r="G47" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G47" s="18"/>
       <c r="H47" s="14" t="s">
         <v>76</v>
       </c>
@@ -4272,9 +4190,7 @@
       <c r="D48" s="15"/>
       <c r="E48" s="16"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G48" s="18"/>
       <c r="H48" s="14" t="s">
         <v>77</v>
       </c>
@@ -4320,9 +4236,7 @@
       <c r="D49" s="15"/>
       <c r="E49" s="16"/>
       <c r="F49" s="18"/>
-      <c r="G49" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G49" s="18"/>
       <c r="H49" s="14" t="s">
         <v>78</v>
       </c>
@@ -4368,9 +4282,7 @@
       <c r="D50" s="15"/>
       <c r="E50" s="16"/>
       <c r="F50" s="18"/>
-      <c r="G50" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G50" s="18"/>
       <c r="H50" s="28" t="s">
         <v>79</v>
       </c>
@@ -4416,9 +4328,7 @@
       <c r="D51" s="15"/>
       <c r="E51" s="16"/>
       <c r="F51" s="18"/>
-      <c r="G51" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="G51" s="18"/>
       <c r="H51" s="28" t="s">
         <v>80</v>
       </c>
@@ -4516,9 +4426,7 @@
       <c r="D53" s="34"/>
       <c r="E53" s="35"/>
       <c r="F53" s="37"/>
-      <c r="G53" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G53" s="37"/>
       <c r="H53" s="36" t="s">
         <v>83</v>
       </c>
@@ -4564,9 +4472,7 @@
       <c r="D54" s="34"/>
       <c r="E54" s="35"/>
       <c r="F54" s="37"/>
-      <c r="G54" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G54" s="37"/>
       <c r="H54" s="44" t="s">
         <v>85</v>
       </c>
@@ -4612,9 +4518,7 @@
       <c r="D55" s="34"/>
       <c r="E55" s="35"/>
       <c r="F55" s="37"/>
-      <c r="G55" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G55" s="37"/>
       <c r="H55" s="44" t="s">
         <v>86</v>
       </c>
@@ -4660,9 +4564,7 @@
       <c r="D56" s="34"/>
       <c r="E56" s="35"/>
       <c r="F56" s="37"/>
-      <c r="G56" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G56" s="37"/>
       <c r="H56" s="44" t="s">
         <v>87</v>
       </c>
@@ -4708,9 +4610,7 @@
       <c r="D57" s="34"/>
       <c r="E57" s="35"/>
       <c r="F57" s="37"/>
-      <c r="G57" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G57" s="37"/>
       <c r="H57" s="44" t="s">
         <v>88</v>
       </c>
@@ -4756,9 +4656,7 @@
       <c r="D58" s="34"/>
       <c r="E58" s="35"/>
       <c r="F58" s="37"/>
-      <c r="G58" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G58" s="37"/>
       <c r="H58" s="44" t="s">
         <v>89</v>
       </c>
@@ -4804,9 +4702,7 @@
       <c r="D59" s="34"/>
       <c r="E59" s="35"/>
       <c r="F59" s="37"/>
-      <c r="G59" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G59" s="37"/>
       <c r="H59" s="44" t="s">
         <v>90</v>
       </c>
@@ -4852,9 +4748,7 @@
       <c r="D60" s="34"/>
       <c r="E60" s="35"/>
       <c r="F60" s="37"/>
-      <c r="G60" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G60" s="37"/>
       <c r="H60" s="44" t="s">
         <v>91</v>
       </c>
@@ -4900,9 +4794,7 @@
       <c r="D61" s="34"/>
       <c r="E61" s="35"/>
       <c r="F61" s="37"/>
-      <c r="G61" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="G61" s="37"/>
       <c r="H61" s="44" t="s">
         <v>92</v>
       </c>

</xml_diff>